<commit_message>
update text to enable downloading by saving image as
</commit_message>
<xml_diff>
--- a/excel_input_template/graphing_template.xlsx
+++ b/excel_input_template/graphing_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yash1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Career\Internships\Bio\Rogulja Lab\Proboscis grahing\excel_input_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5D25A5-BA7C-443D-BBEF-9BE685FE39B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB1D43D-217E-45E1-9701-049A3D72F629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{16EA26FC-6D4B-45B0-97FD-50D5D3222754}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{16EA26FC-6D4B-45B0-97FD-50D5D3222754}"/>
   </bookViews>
   <sheets>
     <sheet name="HOW TO USE" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Group 1</t>
   </si>
@@ -75,12 +75,6 @@
     <t>USAGE INSTRUCTIONS</t>
   </si>
   <si>
-    <t>1. MAKE ONE SHEET PER GROUP</t>
-  </si>
-  <si>
-    <t>2. THE FINAL SHEET SHOULD BE CALLED "SLEEP" AND MARK THE SLEEPING HOURS</t>
-  </si>
-  <si>
     <t>G1 Fly 1 PEs</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
   </si>
   <si>
     <t>G2 Fly 4 PEs</t>
+  </si>
+  <si>
+    <t>https://yashmr.notion.site/Activity-Grapher-64de1a7c9d6347fe87139a00efd367ca</t>
   </si>
 </sst>
 </file>
@@ -112,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[m]:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +120,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -146,17 +152,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81007AEC-9FAD-45A7-99F9-2EBA8B82E76A}">
-  <dimension ref="B2:B5"/>
+  <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,21 +495,14 @@
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <v>3</v>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{D07695BC-78E1-4DD8-A88C-320EDDA11390}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -509,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E872B9-78D6-40CC-A86D-7244C5F07D06}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,7 +611,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>2.0254629629629629E-3</v>
@@ -646,7 +648,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>4.6759259259259263E-3</v>
@@ -669,7 +671,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>2.41203703703704E-2</v>
@@ -691,7 +693,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
         <v>2.0254629629629629E-3</v>
@@ -723,7 +725,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>2.0254629629629629E-3</v>
@@ -759,7 +761,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3">
         <v>4.6759259259259263E-3</v>
@@ -782,7 +784,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3">
         <v>2.41203703703704E-2</v>
@@ -804,7 +806,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3">
         <v>2.0254629629629629E-3</v>
@@ -1094,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA16D3F-2BC5-4512-8484-EAB20F4781C4}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add Pes per hour
</commit_message>
<xml_diff>
--- a/excel_input_template/graphing_template.xlsx
+++ b/excel_input_template/graphing_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Career\Internships\Bio\Rogulja Lab\Proboscis grahing\excel_input_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB1D43D-217E-45E1-9701-049A3D72F629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4469F4BC-D4FA-4F0C-BDA1-2BFF6700E701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{16EA26FC-6D4B-45B0-97FD-50D5D3222754}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{16EA26FC-6D4B-45B0-97FD-50D5D3222754}"/>
   </bookViews>
   <sheets>
     <sheet name="HOW TO USE" sheetId="4" r:id="rId1"/>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E872B9-78D6-40CC-A86D-7244C5F07D06}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,15 +1094,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA16D3F-2BC5-4512-8484-EAB20F4781C4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1135,8 +1135,11 @@
       <c r="E2" s="3">
         <v>0.46609953703703705</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1152,8 +1155,11 @@
       <c r="E3" s="3">
         <v>0.42372685185185183</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1169,8 +1175,11 @@
       <c r="E4" s="3">
         <v>0.46609953703703705</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1186,8 +1195,11 @@
       <c r="E5" s="3">
         <v>0.46609953703703705</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1203,8 +1215,11 @@
       <c r="E6" s="3">
         <v>0.35416666666666669</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1220,8 +1235,11 @@
       <c r="E7" s="3">
         <v>0.42372685185185183</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1237,8 +1255,11 @@
       <c r="E8" s="3">
         <v>0.46609953703703705</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1254,6 +1275,9 @@
       <c r="E9" s="3">
         <v>0.46609953703703705</v>
       </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add shading for sinking
</commit_message>
<xml_diff>
--- a/excel_input_template/graphing_template.xlsx
+++ b/excel_input_template/graphing_template.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Career\Internships\Bio\Rogulja Lab\Proboscis grahing\excel_input_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Career\Internships\Bio\Rogulja Lab\Proboscis grahing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4469F4BC-D4FA-4F0C-BDA1-2BFF6700E701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150A1D43-9E61-42AA-AB17-CBCB51ED885D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{16EA26FC-6D4B-45B0-97FD-50D5D3222754}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{16EA26FC-6D4B-45B0-97FD-50D5D3222754}"/>
   </bookViews>
   <sheets>
     <sheet name="HOW TO USE" sheetId="4" r:id="rId1"/>
     <sheet name="ACTIVITY" sheetId="1" r:id="rId2"/>
     <sheet name="SLEEP" sheetId="5" r:id="rId3"/>
+    <sheet name="SINKING" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>Group 1</t>
   </si>
@@ -512,7 +513,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,15 +1095,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA16D3F-2BC5-4512-8484-EAB20F4781C4}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1135,11 +1136,8 @@
       <c r="E2" s="3">
         <v>0.46609953703703705</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1155,11 +1153,8 @@
       <c r="E3" s="3">
         <v>0.42372685185185183</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1175,11 +1170,8 @@
       <c r="E4" s="3">
         <v>0.46609953703703705</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1195,11 +1187,8 @@
       <c r="E5" s="3">
         <v>0.46609953703703705</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1215,11 +1204,8 @@
       <c r="E6" s="3">
         <v>0.35416666666666669</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1235,11 +1221,8 @@
       <c r="E7" s="3">
         <v>0.42372685185185183</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1255,11 +1238,8 @@
       <c r="E8" s="3">
         <v>0.46609953703703705</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1275,12 +1255,177 @@
       <c r="E9" s="3">
         <v>0.46609953703703705</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F113E6-C19A-4F1C-B04D-1CEE2409F240}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.38194444444444442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.12313657407407408</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.38135416666666666</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.42372685185185183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9.886574074074074E-2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9.886574074074074E-2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.15606481481481482</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.19773148148148148</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.42372685185185183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3">
+        <v>9.886574074074074E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>9.886574074074074E-2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>